<commit_message>
Modify 'main.py' and 'setup.py'
</commit_message>
<xml_diff>
--- a/result/OPTIMAL_COMPLETE_PORTFOLIO_1.xlsx
+++ b/result/OPTIMAL_COMPLETE_PORTFOLIO_1.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
-  <si>
-    <t>GAS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>HPG</t>
   </si>
@@ -457,31 +454,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -492,1255 +489,1036 @@
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="4">
         <v>42858</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:4">
       <c r="A5" s="4">
         <v>42887</v>
       </c>
       <c r="B5">
-        <v>0.009058249288706176</v>
+        <v>0.04122637078783608</v>
       </c>
       <c r="C5">
-        <v>0.04122637078783608</v>
+        <v>-0.009029792457040903</v>
       </c>
       <c r="D5">
-        <v>-0.009029792457040903</v>
-      </c>
-      <c r="E5">
         <v>0.02253684017033791</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:4">
       <c r="A6" s="4">
         <v>42919</v>
       </c>
       <c r="B6">
-        <v>0.08896730042169554</v>
+        <v>0.1633377968849108</v>
       </c>
       <c r="C6">
-        <v>0.1633377968849108</v>
+        <v>-0.05466962051328236</v>
       </c>
       <c r="D6">
-        <v>-0.05466962051328236</v>
-      </c>
-      <c r="E6">
         <v>0.07162572608824294</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:4">
       <c r="A7" s="4">
         <v>42948</v>
       </c>
       <c r="B7">
-        <v>0.07718163514401656</v>
+        <v>-0.009087274181236511</v>
       </c>
       <c r="C7">
-        <v>-0.009087274181236511</v>
+        <v>0.02289308026275821</v>
       </c>
       <c r="D7">
-        <v>0.02289308026275821</v>
-      </c>
-      <c r="E7">
         <v>-0.01285393761052368</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:4">
       <c r="A8" s="4">
         <v>42979</v>
       </c>
       <c r="B8">
-        <v>-0.01090499867319279</v>
+        <v>0.0733893351919102</v>
       </c>
       <c r="C8">
-        <v>0.0733893351919102</v>
+        <v>0.1354516607959012</v>
       </c>
       <c r="D8">
-        <v>0.1354516607959012</v>
-      </c>
-      <c r="E8">
         <v>-0.02473978616441261</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:4">
       <c r="A9" s="4">
         <v>43010</v>
       </c>
       <c r="B9">
-        <v>0.11059303197708</v>
+        <v>0.1125363103035828</v>
       </c>
       <c r="C9">
-        <v>0.1125363103035828</v>
+        <v>0.147303218396109</v>
       </c>
       <c r="D9">
-        <v>0.147303218396109</v>
-      </c>
-      <c r="E9">
         <v>0.02711346343730035</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:4">
       <c r="A10" s="4">
         <v>43040</v>
       </c>
       <c r="B10">
-        <v>0.05035962343133126</v>
+        <v>-0.08578391218872884</v>
       </c>
       <c r="C10">
-        <v>-0.08578391218872884</v>
+        <v>0.08499127360651453</v>
       </c>
       <c r="D10">
-        <v>0.08499127360651453</v>
-      </c>
-      <c r="E10">
         <v>0.1049158658518913</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:4">
       <c r="A11" s="4">
         <v>43070</v>
       </c>
       <c r="B11">
-        <v>0.1348473427891775</v>
+        <v>0.1624554801424636</v>
       </c>
       <c r="C11">
-        <v>0.1624554801424636</v>
+        <v>0.1416669756099571</v>
       </c>
       <c r="D11">
-        <v>0.1416669756099571</v>
-      </c>
-      <c r="E11">
         <v>0.1610582613090402</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:4">
       <c r="A12" s="4">
         <v>43102</v>
       </c>
+      <c r="C12">
+        <v>0.1678828956412398</v>
+      </c>
       <c r="D12">
-        <v>0.1678828956412398</v>
-      </c>
-      <c r="E12">
         <v>0.1387140232025722</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:4">
       <c r="A13" s="4">
         <v>43103</v>
       </c>
       <c r="B13">
-        <v>0.1907080843837415</v>
-      </c>
-      <c r="C13">
         <v>0.1469876964283995</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:4">
       <c r="A14" s="4">
         <v>43132</v>
       </c>
       <c r="B14">
-        <v>0.2546206053468202</v>
+        <v>0.2815190638991323</v>
       </c>
       <c r="C14">
-        <v>0.2815190638991323</v>
+        <v>0.1512509113827066</v>
       </c>
       <c r="D14">
-        <v>0.1512509113827066</v>
-      </c>
-      <c r="E14">
         <v>0.2109104897575042</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:4">
       <c r="A15" s="4">
         <v>43160</v>
       </c>
       <c r="B15">
-        <v>-0.0507368216754894</v>
+        <v>0.09343803462221666</v>
       </c>
       <c r="C15">
-        <v>0.09343803462221666</v>
+        <v>-0.01194311422640801</v>
       </c>
       <c r="D15">
-        <v>-0.01194311422640801</v>
-      </c>
-      <c r="E15">
         <v>0.07357413157190185</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:4">
       <c r="A16" s="4">
         <v>43192</v>
       </c>
       <c r="B16">
-        <v>0.1732756822164733</v>
+        <v>-0.1154385670439286</v>
       </c>
       <c r="C16">
-        <v>-0.1154385670439286</v>
+        <v>0.2593395819017847</v>
       </c>
       <c r="D16">
-        <v>0.2593395819017847</v>
-      </c>
-      <c r="E16">
         <v>0.03496387667821773</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:4">
       <c r="A17" s="4">
         <v>43222</v>
       </c>
       <c r="B17">
-        <v>-0.2380602249924205</v>
+        <v>-0.07796881247501006</v>
       </c>
       <c r="C17">
-        <v>-0.07796881247501006</v>
+        <v>-0.1849906454378313</v>
       </c>
       <c r="D17">
-        <v>-0.1849906454378313</v>
-      </c>
-      <c r="E17">
         <v>-0.2135123616962739</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:4">
       <c r="A18" s="4">
         <v>43252</v>
       </c>
       <c r="B18">
-        <v>-0.1080034679477382</v>
+        <v>0.04779719817131431</v>
       </c>
       <c r="C18">
-        <v>0.04779719817131431</v>
+        <v>-0.1017130125178122</v>
       </c>
       <c r="D18">
-        <v>-0.1017130125178122</v>
-      </c>
-      <c r="E18">
         <v>-0.02062070163886445</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:4">
       <c r="A19" s="4">
         <v>43283</v>
       </c>
       <c r="B19">
-        <v>-0.02262722828553966</v>
+        <v>-0.05686146593993975</v>
       </c>
       <c r="C19">
-        <v>-0.05686146593993975</v>
+        <v>-0.0941602055004359</v>
       </c>
       <c r="D19">
-        <v>-0.0941602055004359</v>
-      </c>
-      <c r="E19">
         <v>0.01929932276115472</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:4">
       <c r="A20" s="4">
         <v>43313</v>
       </c>
       <c r="B20">
-        <v>0.003394295014562353</v>
+        <v>-0.02083286847996675</v>
       </c>
       <c r="C20">
-        <v>-0.02083286847996675</v>
+        <v>0.1078943089430893</v>
       </c>
       <c r="D20">
-        <v>0.1078943089430893</v>
-      </c>
-      <c r="E20">
         <v>0.008606947854446967</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:4">
       <c r="A21" s="4">
         <v>43347</v>
       </c>
       <c r="B21">
-        <v>0.1845527110523001</v>
+        <v>0.03723509304975325</v>
       </c>
       <c r="C21">
-        <v>0.03723509304975325</v>
+        <v>0.1163901343646117</v>
       </c>
       <c r="D21">
-        <v>0.1163901343646117</v>
-      </c>
-      <c r="E21">
         <v>0.0409553523985993</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:4">
       <c r="A22" s="4">
         <v>43374</v>
       </c>
       <c r="B22">
-        <v>0.161165326240448</v>
+        <v>0.08717558146347168</v>
       </c>
       <c r="C22">
-        <v>0.08717558146347168</v>
+        <v>-0.001063552871329819</v>
       </c>
       <c r="D22">
-        <v>-0.001063552871329819</v>
-      </c>
-      <c r="E22">
         <v>0.02458891230274557</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:4">
       <c r="A23" s="4">
         <v>43405</v>
       </c>
       <c r="B23">
-        <v>-0.1513375907365114</v>
+        <v>-0.0660397693592714</v>
       </c>
       <c r="C23">
-        <v>-0.0660397693592714</v>
+        <v>-0.1267304424958116</v>
       </c>
       <c r="D23">
-        <v>-0.1267304424958116</v>
-      </c>
-      <c r="E23">
         <v>-0.1086801933189976</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:4">
       <c r="A24" s="4">
         <v>43437</v>
       </c>
       <c r="B24">
-        <v>-0.04433466576162103</v>
+        <v>-0.1212099356662724</v>
       </c>
       <c r="C24">
-        <v>-0.1212099356662724</v>
+        <v>0.002438388493458691</v>
       </c>
       <c r="D24">
-        <v>0.002438388493458691</v>
-      </c>
-      <c r="E24">
         <v>0.05454515053362753</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:4">
       <c r="A25" s="4">
         <v>43467</v>
       </c>
       <c r="B25">
-        <v>-0.1051552259544157</v>
+        <v>-0.1149401703790029</v>
       </c>
       <c r="C25">
-        <v>-0.1149401703790029</v>
+        <v>-0.04379475352954353</v>
       </c>
       <c r="D25">
-        <v>-0.04379475352954353</v>
-      </c>
-      <c r="E25">
         <v>-0.07586091297660817</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:4">
       <c r="A26" s="4">
         <v>43497</v>
       </c>
       <c r="B26">
-        <v>0.01382497100310544</v>
+        <v>-0.1136395248560381</v>
       </c>
       <c r="C26">
-        <v>-0.1136395248560381</v>
+        <v>-0.002545437393874532</v>
       </c>
       <c r="D26">
-        <v>-0.002545437393874532</v>
-      </c>
-      <c r="E26">
         <v>0.05410453248624959</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:4">
       <c r="A27" s="4">
         <v>43525</v>
       </c>
       <c r="B27">
-        <v>0.1363644751167125</v>
+        <v>0.2545770301090118</v>
       </c>
       <c r="C27">
-        <v>0.2545770301090118</v>
+        <v>0.1352035950890654</v>
       </c>
       <c r="D27">
-        <v>0.1352035950890654</v>
-      </c>
-      <c r="E27">
         <v>0.1008831284791495</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:4">
       <c r="A28" s="4">
         <v>43556</v>
       </c>
       <c r="B28">
-        <v>0.02713063206218787</v>
+        <v>-0.06715310206804542</v>
       </c>
       <c r="C28">
-        <v>-0.06715310206804542</v>
+        <v>-0.01123581464515965</v>
       </c>
       <c r="D28">
-        <v>-0.01123581464515965</v>
-      </c>
-      <c r="E28">
         <v>0.0900331187374326</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:4">
       <c r="A29" s="4">
         <v>43587</v>
       </c>
       <c r="B29">
-        <v>0.1320756634554905</v>
+        <v>0.06416548222442726</v>
       </c>
       <c r="C29">
-        <v>0.06416548222442726</v>
+        <v>0.005681746371672746</v>
       </c>
       <c r="D29">
-        <v>0.005681746371672746</v>
-      </c>
-      <c r="E29">
         <v>-0.01327329026457437</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:4">
       <c r="A30" s="4">
         <v>43619</v>
       </c>
       <c r="B30">
-        <v>-0.1105262475399321</v>
+        <v>-0.07352681758998707</v>
       </c>
       <c r="C30">
-        <v>-0.07352681758998707</v>
+        <v>-0.03954752559166992</v>
       </c>
       <c r="D30">
-        <v>-0.03954752559166992</v>
-      </c>
-      <c r="E30">
         <v>-0.005979686739038309</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:4">
       <c r="A31" s="4">
         <v>43647</v>
       </c>
       <c r="B31">
-        <v>0.02268228760727992</v>
+        <v>-0.05075617451855068</v>
       </c>
       <c r="C31">
-        <v>-0.05075617451855068</v>
+        <v>0.007058440397249925</v>
       </c>
       <c r="D31">
-        <v>0.007058440397249925</v>
-      </c>
-      <c r="E31">
         <v>0.07217999956537123</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:4">
       <c r="A32" s="4">
         <v>43678</v>
       </c>
       <c r="B32">
-        <v>0.04435952123780749</v>
+        <v>-0.01739354690813228</v>
       </c>
       <c r="C32">
-        <v>-0.01739354690813228</v>
+        <v>-0.06425152017370106</v>
       </c>
       <c r="D32">
-        <v>-0.06425152017370106</v>
-      </c>
-      <c r="E32">
         <v>0.129032733571027</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:4">
       <c r="A33" s="4">
         <v>43711</v>
       </c>
       <c r="B33">
-        <v>-0.05727497616517629</v>
+        <v>-0.04203240889251791</v>
       </c>
       <c r="C33">
-        <v>-0.04203240889251791</v>
+        <v>-0.07615500680368674</v>
       </c>
       <c r="D33">
-        <v>-0.07615500680368674</v>
-      </c>
-      <c r="E33">
         <v>-0.03354097884431155</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:4">
       <c r="A34" s="4">
         <v>43739</v>
       </c>
       <c r="B34">
-        <v>0.06412835249042145</v>
+        <v>0.01154755502338932</v>
       </c>
       <c r="C34">
-        <v>0.01154755502338932</v>
+        <v>0.06486466627478224</v>
       </c>
       <c r="D34">
-        <v>0.06486466627478224</v>
-      </c>
-      <c r="E34">
         <v>0.07198015505132634</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:4">
       <c r="A35" s="4">
         <v>43770</v>
       </c>
       <c r="B35">
-        <v>-0.01600766994935206</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>-0.03934083787861207</v>
       </c>
       <c r="D35">
-        <v>-0.03934083787861207</v>
-      </c>
-      <c r="E35">
         <v>0.06474779345858732</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:4">
       <c r="A36" s="4">
         <v>43801</v>
       </c>
       <c r="B36">
-        <v>-0.06220037165349641</v>
+        <v>0.04794005236389901</v>
       </c>
       <c r="C36">
-        <v>0.04794005236389901</v>
+        <v>-0.0885071469149748</v>
       </c>
       <c r="D36">
-        <v>-0.0885071469149748</v>
-      </c>
-      <c r="E36">
         <v>-0.05968457805657472</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:4">
       <c r="A37" s="4">
         <v>43832</v>
       </c>
       <c r="B37">
-        <v>-0.03469415763905499</v>
+        <v>0.04575651408113642</v>
       </c>
       <c r="C37">
-        <v>0.04575651408113642</v>
+        <v>-0.1739126541358097</v>
       </c>
       <c r="D37">
-        <v>-0.1739126541358097</v>
-      </c>
-      <c r="E37">
         <v>0.09708013807903977</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:4">
       <c r="A38" s="4">
         <v>43864</v>
       </c>
       <c r="B38">
-        <v>-0.120507508880113</v>
+        <v>0.02291159401717219</v>
       </c>
       <c r="C38">
-        <v>0.02291159401717219</v>
+        <v>-0.1228075880758807</v>
       </c>
       <c r="D38">
-        <v>-0.1228075880758807</v>
-      </c>
-      <c r="E38">
         <v>-0.02312844194584657</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:4">
       <c r="A39" s="4">
         <v>43892</v>
       </c>
       <c r="B39">
-        <v>-0.05048096192384762</v>
+        <v>-0.09165182686198522</v>
       </c>
       <c r="C39">
-        <v>-0.09165182686198522</v>
+        <v>-0.01999975284536781</v>
       </c>
       <c r="D39">
-        <v>-0.01999975284536781</v>
-      </c>
-      <c r="E39">
         <v>-0.07779015874553886</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:4">
       <c r="A40" s="4">
         <v>43922</v>
       </c>
       <c r="B40">
-        <v>-0.2898728744996236</v>
+        <v>-0.2264572886598954</v>
       </c>
       <c r="C40">
-        <v>-0.2264572886598954</v>
+        <v>0.004083094375216016</v>
       </c>
       <c r="D40">
-        <v>0.004083094375216016</v>
-      </c>
-      <c r="E40">
         <v>-0.2053788329836381</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:4">
       <c r="A41" s="4">
         <v>43955</v>
       </c>
       <c r="B41">
-        <v>0.1372543580517458</v>
+        <v>0.2173968415690269</v>
       </c>
       <c r="C41">
-        <v>0.2173968415690269</v>
+        <v>0.1646338400329539</v>
       </c>
       <c r="D41">
-        <v>0.1646338400329539</v>
-      </c>
-      <c r="E41">
         <v>0.03692247282401831</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:4">
       <c r="A42" s="4">
         <v>43983</v>
       </c>
       <c r="B42">
-        <v>0.1802515810930886</v>
+        <v>0.316664923109112</v>
       </c>
       <c r="C42">
-        <v>0.316664923109112</v>
+        <v>0.1012211060261646</v>
       </c>
       <c r="D42">
-        <v>0.1012211060261646</v>
-      </c>
-      <c r="E42">
         <v>0.2833839531361093</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:4">
       <c r="A43" s="4">
         <v>44013</v>
       </c>
       <c r="B43">
-        <v>-0.05710561549623656</v>
+        <v>-0.009041792467821346</v>
       </c>
       <c r="C43">
-        <v>-0.009041792467821346</v>
+        <v>-0.1204437028506968</v>
       </c>
       <c r="D43">
-        <v>-0.1204437028506968</v>
-      </c>
-      <c r="E43">
         <v>-0.04393165918715439</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:4">
       <c r="A44" s="4">
         <v>44046</v>
       </c>
       <c r="B44">
-        <v>-0.007154666032087984</v>
+        <v>0.0215920206539343</v>
       </c>
       <c r="C44">
-        <v>0.0215920206539343</v>
+        <v>-0.05225199950123796</v>
       </c>
       <c r="D44">
-        <v>-0.05225199950123796</v>
-      </c>
-      <c r="E44">
         <v>-0.04715806114849067</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:4">
       <c r="A45" s="4">
         <v>44075</v>
       </c>
       <c r="B45">
-        <v>0.1220232932917464</v>
+        <v>0.08297296236706823</v>
       </c>
       <c r="C45">
-        <v>0.08297296236706823</v>
+        <v>0.03802229557495081</v>
       </c>
       <c r="D45">
-        <v>0.03802229557495081</v>
-      </c>
-      <c r="E45">
         <v>0.05329946722015845</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:4">
       <c r="A46" s="4">
         <v>44105</v>
       </c>
       <c r="B46">
-        <v>-0.03978733989358552</v>
+        <v>0.08871125540811815</v>
       </c>
       <c r="C46">
-        <v>0.08871125540811815</v>
+        <v>0.005495338694381822</v>
       </c>
       <c r="D46">
-        <v>0.005495338694381822</v>
-      </c>
-      <c r="E46">
         <v>0.02168718552953415</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:4">
       <c r="A47" s="4">
         <v>44137</v>
       </c>
       <c r="B47">
-        <v>-0.03729398006870143</v>
+        <v>0.1333306707138483</v>
       </c>
       <c r="C47">
-        <v>0.1333306707138483</v>
+        <v>0.5391608911058238</v>
       </c>
       <c r="D47">
-        <v>0.5391608911058238</v>
-      </c>
-      <c r="E47">
         <v>0.01179200373462075</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:4">
       <c r="A48" s="4">
         <v>44166</v>
       </c>
       <c r="B48">
-        <v>0.1979929032513081</v>
+        <v>0.1633990766953682</v>
       </c>
       <c r="C48">
-        <v>0.1633990766953682</v>
+        <v>-0.01775124564372019</v>
       </c>
       <c r="D48">
-        <v>-0.01775124564372019</v>
-      </c>
-      <c r="E48">
         <v>0.07226169137768014</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:4">
       <c r="A49" s="4">
         <v>44200</v>
       </c>
       <c r="B49">
-        <v>0.06347216176670288</v>
+        <v>0.1882036369511</v>
       </c>
       <c r="C49">
-        <v>0.1882036369511</v>
+        <v>0.08387317705037618</v>
       </c>
       <c r="D49">
-        <v>0.08387317705037618</v>
-      </c>
-      <c r="E49">
         <v>0.08487391984373549</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:4">
       <c r="A50" s="4">
         <v>44228</v>
       </c>
       <c r="B50">
-        <v>-0.1531523898736896</v>
+        <v>-0.09338154378242404</v>
       </c>
       <c r="C50">
-        <v>-0.09338154378242404</v>
+        <v>-0.07761498287036145</v>
       </c>
       <c r="D50">
-        <v>-0.07761498287036145</v>
-      </c>
-      <c r="E50">
         <v>-0.07979824073856615</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:4">
       <c r="A51" s="4">
         <v>44256</v>
       </c>
       <c r="B51">
-        <v>0.2220733269360028</v>
+        <v>0.2046968070897323</v>
       </c>
       <c r="C51">
-        <v>0.2046968070897323</v>
+        <v>0.1134143290303748</v>
       </c>
       <c r="D51">
-        <v>0.1134143290303748</v>
-      </c>
-      <c r="E51">
         <v>0.08891302375172978</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:4">
       <c r="A52" s="4">
         <v>44287</v>
       </c>
       <c r="B52">
-        <v>-0.01414553714529497</v>
+        <v>0.04978273301252244</v>
       </c>
       <c r="C52">
-        <v>0.04978273301252244</v>
+        <v>0.01095326437774784</v>
       </c>
       <c r="D52">
-        <v>0.01095326437774784</v>
-      </c>
-      <c r="E52">
         <v>-0.0231847147027498</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:4">
       <c r="A53" s="4">
         <v>44320</v>
       </c>
       <c r="B53">
-        <v>-0.08057408052846675</v>
+        <v>0.2329889495801434</v>
       </c>
       <c r="C53">
-        <v>0.2329889495801434</v>
+        <v>0.03900267259400392</v>
       </c>
       <c r="D53">
-        <v>0.03900267259400392</v>
-      </c>
-      <c r="E53">
         <v>0.02270327912556664</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:4">
       <c r="A54" s="4">
         <v>44348</v>
       </c>
       <c r="B54">
-        <v>0.0048021208200879</v>
+        <v>0.2623682478428261</v>
       </c>
       <c r="C54">
-        <v>0.2623682478428261</v>
+        <v>0.115745722329966</v>
       </c>
       <c r="D54">
-        <v>0.115745722329966</v>
-      </c>
-      <c r="E54">
         <v>0.04641751126126111</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:4">
       <c r="A55" s="4">
         <v>44378</v>
       </c>
       <c r="B55">
-        <v>0.1609738620509794</v>
+        <v>-0.04864960097518233</v>
       </c>
       <c r="C55">
-        <v>-0.04864960097518233</v>
+        <v>0.06984183867956185</v>
       </c>
       <c r="D55">
-        <v>0.06984183867956185</v>
-      </c>
-      <c r="E55">
         <v>0.1224694679545866</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:4">
       <c r="A56" s="4">
         <v>44410</v>
       </c>
       <c r="B56">
-        <v>-0.007430452642586902</v>
+        <v>-0.1051127405590731</v>
       </c>
       <c r="C56">
-        <v>-0.1051127405590731</v>
+        <v>0.200000213358595</v>
       </c>
       <c r="D56">
-        <v>0.200000213358595</v>
-      </c>
-      <c r="E56">
         <v>-0.166666851611629</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:4">
       <c r="A57" s="4">
         <v>44440</v>
       </c>
       <c r="B57">
-        <v>-0.05240693764055624</v>
+        <v>0.04127095987561102</v>
       </c>
       <c r="C57">
-        <v>0.04127095987561102</v>
+        <v>-0.02129229500020891</v>
       </c>
       <c r="D57">
-        <v>-0.02129229500020891</v>
-      </c>
-      <c r="E57">
         <v>0.02474253436204193</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:4">
       <c r="A58" s="4">
         <v>44470</v>
       </c>
       <c r="B58">
-        <v>0.1681721372581074</v>
+        <v>0.08536415054814607</v>
       </c>
       <c r="C58">
-        <v>0.08536415054814607</v>
+        <v>0.05026269034149747</v>
       </c>
       <c r="D58">
-        <v>0.05026269034149747</v>
-      </c>
-      <c r="E58">
         <v>-0.03521125845456138</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:4">
       <c r="A59" s="4">
         <v>44501</v>
       </c>
       <c r="B59">
-        <v>0.1719805909844745</v>
+        <v>0.04307266703123484</v>
       </c>
       <c r="C59">
-        <v>0.04307266703123484</v>
+        <v>0.03928558764489717</v>
       </c>
       <c r="D59">
-        <v>0.03928558764489717</v>
-      </c>
-      <c r="E59">
         <v>0.01147000907795445</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:4">
       <c r="A60" s="4">
         <v>44531</v>
       </c>
       <c r="B60">
-        <v>-0.1879636467105219</v>
+        <v>-0.1202880879066656</v>
       </c>
       <c r="C60">
-        <v>-0.1202880879066656</v>
+        <v>0.03024028959577254</v>
       </c>
       <c r="D60">
-        <v>0.03024028959577254</v>
-      </c>
-      <c r="E60">
         <v>0.02061855670103094</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:4">
       <c r="A61" s="4">
         <v>44565</v>
       </c>
       <c r="B61">
-        <v>0.03451774849879772</v>
+        <v>-0.04591836734693868</v>
       </c>
       <c r="C61">
-        <v>-0.04591836734693868</v>
+        <v>0.1359071868331053</v>
       </c>
       <c r="D61">
-        <v>0.1359071868331053</v>
-      </c>
-      <c r="E61">
         <v>0.03071531642960222</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:4">
       <c r="A62" s="4">
         <v>44599</v>
       </c>
       <c r="B62">
-        <v>0.1256132831046867</v>
+        <v>-0.07914551559620592</v>
       </c>
       <c r="C62">
-        <v>-0.07914551559620592</v>
+        <v>-0.1300000213330451</v>
       </c>
       <c r="D62">
-        <v>-0.1300000213330451</v>
-      </c>
-      <c r="E62">
         <v>0.169620253164557</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:4">
       <c r="A63" s="4">
         <v>44621</v>
       </c>
       <c r="B63">
-        <v>0.02615517573358532</v>
+        <v>0.08943161797656242</v>
       </c>
       <c r="C63">
-        <v>0.08943161797656242</v>
+        <v>0.05814685308969516</v>
       </c>
       <c r="D63">
-        <v>0.05814685308969516</v>
-      </c>
-      <c r="E63">
         <v>-0.08008658008658014</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:4">
       <c r="A64" s="4">
         <v>44652</v>
       </c>
       <c r="B64">
-        <v>-0.06796938410382172</v>
+        <v>-0.02558467793057392</v>
       </c>
       <c r="C64">
-        <v>-0.02558467793057392</v>
+        <v>-0.0638972527294271</v>
       </c>
       <c r="D64">
-        <v>-0.0638972527294271</v>
-      </c>
-      <c r="E64">
         <v>-0.02588235294117651</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:4">
       <c r="A65" s="4">
         <v>44685</v>
       </c>
       <c r="B65">
-        <v>-0.01549727042034591</v>
+        <v>-0.0809638637822459</v>
       </c>
       <c r="C65">
-        <v>-0.0809638637822459</v>
+        <v>-0.07354648548156444</v>
       </c>
       <c r="D65">
-        <v>-0.07354648548156444</v>
-      </c>
-      <c r="E65">
         <v>-0.03502415458937188</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:4">
       <c r="A66" s="4">
         <v>44713</v>
       </c>
       <c r="B66">
-        <v>0.1203703703703703</v>
+        <v>-0.1821422279271117</v>
       </c>
       <c r="C66">
-        <v>-0.1821422279271117</v>
+        <v>0.01679902097005194</v>
       </c>
       <c r="D66">
-        <v>0.01679902097005194</v>
-      </c>
-      <c r="E66">
         <v>0.0075093867334167</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:4">
       <c r="A67" s="4">
         <v>44743</v>
       </c>
       <c r="B67">
-        <v>-0.06611570247933882</v>
+        <v>-0.1383322883047842</v>
       </c>
       <c r="C67">
-        <v>-0.1383322883047842</v>
+        <v>-0.04782564897666006</v>
       </c>
       <c r="D67">
-        <v>-0.04782564897666006</v>
-      </c>
-      <c r="E67">
         <v>-0.08074534161490683</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:4">
       <c r="A68" s="4">
         <v>44774</v>
       </c>
       <c r="B68">
-        <v>-0.01913995209330436</v>
+        <v>0.01785714285714295</v>
       </c>
       <c r="C68">
-        <v>0.01785714285714295</v>
+        <v>0.006433261239348119</v>
       </c>
       <c r="D68">
-        <v>0.006433261239348119</v>
-      </c>
-      <c r="E68">
         <v>0.04054054054054054</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:4">
       <c r="A69" s="4">
         <v>44809</v>
       </c>
       <c r="B69">
-        <v>0.07877664504170528</v>
+        <v>0.04824561403508763</v>
       </c>
       <c r="C69">
-        <v>0.04824561403508763</v>
+        <v>0.05575868372943322</v>
       </c>
       <c r="D69">
-        <v>0.05575868372943322</v>
-      </c>
-      <c r="E69">
         <v>0.07272727272727265</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:4">
       <c r="A70" s="4">
         <v>44837</v>
       </c>
       <c r="B70">
-        <v>-0.08075601374570451</v>
+        <v>-0.1736401673640167</v>
       </c>
       <c r="C70">
-        <v>-0.1736401673640167</v>
+        <v>-0.1861471861471861</v>
       </c>
       <c r="D70">
-        <v>-0.1861471861471861</v>
-      </c>
-      <c r="E70">
         <v>-0.1452784503631961</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:4">
       <c r="A71" s="4">
         <v>44866</v>
       </c>
       <c r="B71">
-        <v>0.02803738317757009</v>
+        <v>-0.2405063291139241</v>
       </c>
       <c r="C71">
-        <v>-0.2405063291139241</v>
+        <v>-0.0797872340425532</v>
       </c>
       <c r="D71">
-        <v>-0.0797872340425532</v>
-      </c>
-      <c r="E71">
         <v>0.06232294617563748</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:4">
       <c r="A72" s="4">
         <v>44896</v>
       </c>
       <c r="B72">
-        <v>-0.03181818181818181</v>
+        <v>0.2133333333333333</v>
       </c>
       <c r="C72">
-        <v>0.2133333333333333</v>
+        <v>0.1445086705202312</v>
       </c>
       <c r="D72">
-        <v>0.1445086705202312</v>
-      </c>
-      <c r="E72">
         <v>0.06666666666666667</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:4">
       <c r="A73" s="4">
         <v>44929</v>
       </c>
       <c r="B73">
-        <v>-0.01408450704225352</v>
+        <v>0.05769230769230773</v>
       </c>
       <c r="C73">
-        <v>0.05769230769230773</v>
+        <v>-0.0303030303030303</v>
       </c>
       <c r="D73">
-        <v>-0.0303030303030303</v>
-      </c>
-      <c r="E73">
         <v>0.03249999999999993</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:4">
       <c r="A74" s="4">
         <v>44958</v>
       </c>
       <c r="B74">
-        <v>0.01523809523809518</v>
+        <v>0.09610389610389618</v>
       </c>
       <c r="C74">
-        <v>0.09610389610389618</v>
+        <v>-0.008333333333333304</v>
       </c>
       <c r="D74">
-        <v>-0.008333333333333304</v>
-      </c>
-      <c r="E74">
         <v>0.07869249394673124</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:4">
       <c r="A75" s="4">
         <v>44986</v>
       </c>
       <c r="B75">
-        <v>-0.01407129455909944</v>
+        <v>-0.009478672985782125</v>
       </c>
       <c r="C75">
-        <v>-0.009478672985782125</v>
+        <v>-0.1544117647058824</v>
       </c>
       <c r="D75">
-        <v>-0.1544117647058824</v>
-      </c>
-      <c r="E75">
         <v>0.04377104377104384</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:4">
       <c r="A76" s="4">
         <v>45019</v>
       </c>
       <c r="B76">
-        <v>-0.02473834443387245</v>
+        <v>0.004784688995215379</v>
       </c>
       <c r="C76">
-        <v>0.004784688995215379</v>
+        <v>-0.04596273291925469</v>
       </c>
       <c r="D76">
-        <v>-0.04596273291925469</v>
-      </c>
-      <c r="E76">
         <v>-0.002150537634408633</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:4">
       <c r="A77" s="4">
         <v>45050</v>
       </c>
       <c r="B77">
-        <v>-0.1024390243902439</v>
+        <v>0.01428571428571432</v>
       </c>
       <c r="C77">
-        <v>0.01428571428571432</v>
+        <v>-0.08072916666666671</v>
       </c>
       <c r="D77">
-        <v>-0.08072916666666671</v>
-      </c>
-      <c r="E77">
         <v>-0.04633620689655169</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:4">
       <c r="B79" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B80">
-        <v>0.0165</v>
+        <v>0.0231</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1748,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="B81">
-        <v>0.0231</v>
+        <v>0.0155</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1756,232 +1534,187 @@
         <v>2</v>
       </c>
       <c r="B82">
-        <v>0.0155</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83">
         <v>0.0207</v>
       </c>
     </row>
+    <row r="84" spans="1:5">
+      <c r="B84" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="85" spans="1:5">
-      <c r="B85" s="3" t="s">
+      <c r="A85" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>3</v>
+      <c r="B85">
+        <v>0.01474321812124414</v>
+      </c>
+      <c r="C85">
+        <v>0.005495049977468246</v>
+      </c>
+      <c r="D85">
+        <v>0.005163119843702485</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B86">
-        <v>0.01217212353952003</v>
+        <v>0.005495049977468246</v>
       </c>
       <c r="C86">
-        <v>0.006388202423926582</v>
+        <v>0.013131852740586</v>
       </c>
       <c r="D86">
-        <v>0.005322613980077881</v>
-      </c>
-      <c r="E86">
-        <v>0.00606689209750367</v>
+        <v>0.002813917623351446</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87">
+        <v>0.005163119843702485</v>
+      </c>
+      <c r="C87">
+        <v>0.002813917623351446</v>
+      </c>
+      <c r="D87">
+        <v>0.00728941374692255</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="B90" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91">
+        <v>0.2415252624007518</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B87">
-        <v>0.006388202423926582</v>
-      </c>
-      <c r="C87">
-        <v>0.01474321812124414</v>
-      </c>
-      <c r="D87">
-        <v>0.005495049977468246</v>
-      </c>
-      <c r="E87">
-        <v>0.005163119843702485</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88">
-        <v>0.005322613980077881</v>
-      </c>
-      <c r="C88">
-        <v>0.005495049977468246</v>
-      </c>
-      <c r="D88">
-        <v>0.013131852740586</v>
-      </c>
-      <c r="E88">
-        <v>0.002813917623351446</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B89">
-        <v>0.00606689209750367</v>
-      </c>
-      <c r="C89">
-        <v>0.005163119843702485</v>
-      </c>
-      <c r="D89">
-        <v>0.002813917623351446</v>
-      </c>
-      <c r="E89">
-        <v>0.00728941374692255</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="B92" s="3" t="s">
-        <v>8</v>
+      <c r="B92">
+        <v>0.07073319353818125</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B93">
-        <v>0.05000000000000006</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
-      <c r="A94" s="3" t="s">
+        <v>0.6877415440610669</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="B96" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="3">
         <v>0</v>
       </c>
-      <c r="B94">
-        <v>0.237872326605806</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B95">
-        <v>0.05769687012930377</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
-      <c r="A96" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B96">
-        <v>0.6544308032648902</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="1" t="s">
+      <c r="B97">
+        <v>0.02091184802336326</v>
+      </c>
+      <c r="C97">
+        <v>0.08093412795536611</v>
+      </c>
+      <c r="D97">
+        <v>0.005833333333333334</v>
+      </c>
+      <c r="E97">
+        <v>0.1863</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="B100" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="B99" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C99" s="3" t="s">
+      <c r="B101">
+        <v>0.1278859031860413</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B102">
+        <v>0.8721140968139587</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="B105" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="3">
+      <c r="E105" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="3">
         <v>0</v>
       </c>
-      <c r="B100">
-        <v>0.02076086985918156</v>
-      </c>
-      <c r="C100">
-        <v>0.08112215677775718</v>
-      </c>
-      <c r="D100">
+      <c r="B106">
+        <v>0.007761662803171801</v>
+      </c>
+      <c r="C106">
+        <v>0.01035033405214663</v>
+      </c>
+      <c r="D106">
         <v>0.005833333333333334</v>
       </c>
-      <c r="E100">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
-      <c r="B103" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
-      <c r="A104" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B104">
-        <v>0.1260191831284673</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
-      <c r="A105" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B105">
-        <v>0.8739808168715327</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
-      <c r="A107" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="B108" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="3">
-        <v>0</v>
-      </c>
-      <c r="B109">
-        <v>0.007714489292441085</v>
-      </c>
-      <c r="C109">
-        <v>0.01022294793075241</v>
-      </c>
-      <c r="D109">
-        <v>0.005833333333333334</v>
-      </c>
-      <c r="E109">
+      <c r="E106">
         <v>0.0068</v>
       </c>
     </row>
@@ -1989,8 +1722,8 @@
   <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="A104:D104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>